<commit_message>
fixed small issues and cleaning of output
</commit_message>
<xml_diff>
--- a/LOGS/89310a5f-45fc-4d11-bcc1-661a581e3891/main_page_service_output/notes_cropped_df.xlsx
+++ b/LOGS/89310a5f-45fc-4d11-bcc1-661a581e3891/main_page_service_output/notes_cropped_df.xlsx
@@ -11,28 +11,33 @@
     <sheet name="7__783d1f36-c06c-341" sheetId="2" r:id="rId2"/>
     <sheet name="8__783d1f36-c06c-341" sheetId="3" r:id="rId3"/>
     <sheet name="9__6354e3c7-4619-3a0" sheetId="4" r:id="rId4"/>
-    <sheet name="11__09af3f09-68b9-35" sheetId="5" r:id="rId5"/>
-    <sheet name="11__e3601430-2dd6-33" sheetId="6" r:id="rId6"/>
-    <sheet name="11__bb79b34d-1e9c-34" sheetId="7" r:id="rId7"/>
-    <sheet name="12__24662bf7-9672-32" sheetId="8" r:id="rId8"/>
-    <sheet name="16__2307c038-33fd-3b" sheetId="9" r:id="rId9"/>
-    <sheet name="16__6bafd8f6-8a94-32" sheetId="10" r:id="rId10"/>
-    <sheet name="17__65990df0-8285-3b" sheetId="11" r:id="rId11"/>
-    <sheet name="15__2307c038-33fd-3b" sheetId="12" r:id="rId12"/>
-    <sheet name="18__8a5d8593-402f-32" sheetId="13" r:id="rId13"/>
-    <sheet name="19__85574d29-1138-3d" sheetId="14" r:id="rId14"/>
-    <sheet name="4_1_e8b583fe-7a0d-33" sheetId="15" r:id="rId15"/>
-    <sheet name="4_2_e8b583fe-7a0d-33" sheetId="16" r:id="rId16"/>
-    <sheet name="4_3_e8b583fe-7a0d-33" sheetId="17" r:id="rId17"/>
-    <sheet name="4_4_dfb38738-8ae6-35" sheetId="18" r:id="rId18"/>
-    <sheet name="4_5_dfb38738-8ae6-35" sheetId="19" r:id="rId19"/>
+    <sheet name="20__817597a4-1bac-38" sheetId="5" r:id="rId5"/>
+    <sheet name="11__09af3f09-68b9-35" sheetId="6" r:id="rId6"/>
+    <sheet name="11__e3601430-2dd6-33" sheetId="7" r:id="rId7"/>
+    <sheet name="11__bb79b34d-1e9c-34" sheetId="8" r:id="rId8"/>
+    <sheet name="12__24662bf7-9672-32" sheetId="9" r:id="rId9"/>
+    <sheet name="5__be4d92ca-40d3-32d" sheetId="10" r:id="rId10"/>
+    <sheet name="5__994bc063-83b4-3b8" sheetId="11" r:id="rId11"/>
+    <sheet name="5__673995c5-d2ab-3ea" sheetId="12" r:id="rId12"/>
+    <sheet name="5__67dae025-9104-3cc" sheetId="13" r:id="rId13"/>
+    <sheet name="16__2307c038-33fd-3b" sheetId="14" r:id="rId14"/>
+    <sheet name="16__6bafd8f6-8a94-32" sheetId="15" r:id="rId15"/>
+    <sheet name="17__65990df0-8285-3b" sheetId="16" r:id="rId16"/>
+    <sheet name="15__2307c038-33fd-3b" sheetId="17" r:id="rId17"/>
+    <sheet name="18__8a5d8593-402f-32" sheetId="18" r:id="rId18"/>
+    <sheet name="19__85574d29-1138-3d" sheetId="19" r:id="rId19"/>
+    <sheet name="4_1_e8b583fe-7a0d-33" sheetId="20" r:id="rId20"/>
+    <sheet name="4_2_e8b583fe-7a0d-33" sheetId="21" r:id="rId21"/>
+    <sheet name="4_3_e8b583fe-7a0d-33" sheetId="22" r:id="rId22"/>
+    <sheet name="4_4_dfb38738-8ae6-35" sheetId="23" r:id="rId23"/>
+    <sheet name="4_5_dfb38738-8ae6-35" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="366">
   <si>
     <t>6. Cash and cash equivalents</t>
   </si>
@@ -139,6 +144,84 @@
     <t>12453</t>
   </si>
   <si>
+    <t>Ultimate parent</t>
+  </si>
+  <si>
+    <t>Marubeni Corporation</t>
+  </si>
+  <si>
+    <t>Other related parties</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Sales to related parties</t>
+  </si>
+  <si>
+    <t>190813761</t>
+  </si>
+  <si>
+    <t>24096896</t>
+  </si>
+  <si>
+    <t>214910657</t>
+  </si>
+  <si>
+    <t>Management and Service</t>
+  </si>
+  <si>
+    <t>fees to</t>
+  </si>
+  <si>
+    <t>related</t>
+  </si>
+  <si>
+    <t>parties</t>
+  </si>
+  <si>
+    <t>1758031</t>
+  </si>
+  <si>
+    <t>138000</t>
+  </si>
+  <si>
+    <t>1896031</t>
+  </si>
+  <si>
+    <t>Income tax receivable from related parties</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>6318000</t>
+  </si>
+  <si>
+    <t>Amounts owed by related parties*</t>
+  </si>
+  <si>
+    <t>10603755</t>
+  </si>
+  <si>
+    <t>1322964</t>
+  </si>
+  <si>
+    <t>11926719</t>
+  </si>
+  <si>
+    <t>Amounts owed to related parties*</t>
+  </si>
+  <si>
+    <t>3784111</t>
+  </si>
+  <si>
+    <t>4627015</t>
+  </si>
+  <si>
+    <t>8411126</t>
+  </si>
+  <si>
     <t>Name of entity</t>
   </si>
   <si>
@@ -361,9 +444,6 @@
     <t>1678</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>408777</t>
   </si>
   <si>
@@ -394,6 +474,291 @@
     <t>3731</t>
   </si>
   <si>
+    <t>Current income tax:</t>
+  </si>
+  <si>
+    <t>Current income tax benefit</t>
+  </si>
+  <si>
+    <t>Adjustments in respect of current income tax of previous year</t>
+  </si>
+  <si>
+    <t>Deferred income tax:</t>
+  </si>
+  <si>
+    <t>Origination and reversal of temporary differences</t>
+  </si>
+  <si>
+    <t>Income tax benefit reported in the statement of profit or loss and other</t>
+  </si>
+  <si>
+    <t>comprehensive income</t>
+  </si>
+  <si>
+    <t>5119</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>3027</t>
+  </si>
+  <si>
+    <t>8217</t>
+  </si>
+  <si>
+    <t>5473</t>
+  </si>
+  <si>
+    <t>(1,529)</t>
+  </si>
+  <si>
+    <t>3944</t>
+  </si>
+  <si>
+    <t>5. Income tax (continued)</t>
+  </si>
+  <si>
+    <t>Accounting loss before income tax</t>
+  </si>
+  <si>
+    <t>At Australia's statutory income tax rate of 30% (2019: 30%)</t>
+  </si>
+  <si>
+    <t>Amounts not deductible for tax purposes</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Income tax benefit reported in profit or loss</t>
+  </si>
+  <si>
+    <t>(28,082)</t>
+  </si>
+  <si>
+    <t>8425</t>
+  </si>
+  <si>
+    <t>(192)</t>
+  </si>
+  <si>
+    <t>(87)</t>
+  </si>
+  <si>
+    <t>(8,217)</t>
+  </si>
+  <si>
+    <t>(20,678)</t>
+  </si>
+  <si>
+    <t>6203</t>
+  </si>
+  <si>
+    <t>(2,276)</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>(3,944)</t>
+  </si>
+  <si>
+    <t>As of 1 January</t>
+  </si>
+  <si>
+    <t>Income tax benefit during the year recognised in profit or loss</t>
+  </si>
+  <si>
+    <t>Income tax benefit during the year recognised in other comprehensive income</t>
+  </si>
+  <si>
+    <t>As at 31 December</t>
+  </si>
+  <si>
+    <t>(11,017)</t>
+  </si>
+  <si>
+    <t>13747</t>
+  </si>
+  <si>
+    <t>5757</t>
+  </si>
+  <si>
+    <t>(14,534)</t>
+  </si>
+  <si>
+    <t>5046</t>
+  </si>
+  <si>
+    <t>Financial assets</t>
+  </si>
+  <si>
+    <t>Property, plant and equipment</t>
+  </si>
+  <si>
+    <t>Right-of-use assets</t>
+  </si>
+  <si>
+    <t>Other assets</t>
+  </si>
+  <si>
+    <t>Trade and other payables</t>
+  </si>
+  <si>
+    <t>Provisions</t>
+  </si>
+  <si>
+    <t>Lease liabilities</t>
+  </si>
+  <si>
+    <t>Financial liabilities</t>
+  </si>
+  <si>
+    <t>ARO assets</t>
+  </si>
+  <si>
+    <t>Deferred tax benefit</t>
+  </si>
+  <si>
+    <t>Net deferred tax assets/liabilities)</t>
+  </si>
+  <si>
+    <t>Reflected in the statement of financial position</t>
+  </si>
+  <si>
+    <t>as follows:</t>
+  </si>
+  <si>
+    <t>Deferred tax assets</t>
+  </si>
+  <si>
+    <t>Deferred tax liabilities</t>
+  </si>
+  <si>
+    <t>Deferred tax assets/liabilities), net</t>
+  </si>
+  <si>
+    <t>Statement of profit or loss Statement of financial and other comprehensive position income</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>6559</t>
+  </si>
+  <si>
+    <t>(302)</t>
+  </si>
+  <si>
+    <t>(13,952)</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>16238</t>
+  </si>
+  <si>
+    <t>316</t>
+  </si>
+  <si>
+    <t>881</t>
+  </si>
+  <si>
+    <t>(4,213)</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>24223</t>
+  </si>
+  <si>
+    <t>(18,466)</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>(12,662)</t>
+  </si>
+  <si>
+    <t>7055</t>
+  </si>
+  <si>
+    <t>(443)</t>
+  </si>
+  <si>
+    <t>(10,221)</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>4671</t>
+  </si>
+  <si>
+    <t>454</t>
+  </si>
+  <si>
+    <t>12309</t>
+  </si>
+  <si>
+    <t>(23,326)</t>
+  </si>
+  <si>
+    <t>496</t>
+  </si>
+  <si>
+    <t>(141)</t>
+  </si>
+  <si>
+    <t>3730</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>(11,567)</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>(881)</t>
+  </si>
+  <si>
+    <t>4213</t>
+  </si>
+  <si>
+    <t>(162)</t>
+  </si>
+  <si>
+    <t>(16,775)</t>
+  </si>
+  <si>
+    <t>5181</t>
+  </si>
+  <si>
+    <t>(1,034)</t>
+  </si>
+  <si>
+    <t>(12)</t>
+  </si>
+  <si>
+    <t>(643)</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>(79)</t>
+  </si>
+  <si>
+    <t>3517</t>
+  </si>
+  <si>
     <t>16. Borrowings</t>
   </si>
   <si>
@@ -547,13 +912,7 @@
     <t>15. Financial liabilities</t>
   </si>
   <si>
-    <t>Trade and other payables</t>
-  </si>
-  <si>
     <t>Electricity derivatives at fair value through OCI</t>
-  </si>
-  <si>
-    <t>Lease liabilities</t>
   </si>
   <si>
     <t>25569</t>
@@ -1205,6 +1564,653 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D7" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" t="s">
+        <v>229</v>
+      </c>
+      <c r="E13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" t="s">
+        <v>232</v>
+      </c>
+      <c r="E16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1241,16 +2247,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="C3" t="s">
-        <v>127</v>
+        <v>247</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>251</v>
       </c>
       <c r="E3" t="s">
-        <v>127</v>
+        <v>247</v>
       </c>
       <c r="F3" t="s">
-        <v>131</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1269,64 +2275,64 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>243</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>243</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>252</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>244</v>
       </c>
       <c r="E6" t="s">
-        <v>122</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>246</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>249</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>252</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>253</v>
       </c>
       <c r="F7" t="s">
-        <v>132</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>245</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="E8" t="s">
-        <v>134</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -1334,7 +2340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -1367,102 +2373,102 @@
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
-        <v>138</v>
+        <v>258</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>264</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>268</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
+        <v>272</v>
       </c>
       <c r="F2" t="s">
-        <v>157</v>
+        <v>277</v>
       </c>
       <c r="G2" t="s">
-        <v>163</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>259</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>265</v>
       </c>
       <c r="E3" t="s">
-        <v>153</v>
+        <v>273</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>278</v>
       </c>
       <c r="G3" t="s">
-        <v>164</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>255</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>260</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>266</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>269</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>274</v>
       </c>
       <c r="F4" t="s">
-        <v>159</v>
+        <v>279</v>
       </c>
       <c r="G4" t="s">
-        <v>165</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>256</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>270</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>275</v>
       </c>
       <c r="G5" t="s">
-        <v>166</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>257</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>267</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>271</v>
       </c>
       <c r="E6" t="s">
-        <v>156</v>
+        <v>276</v>
       </c>
       <c r="F6" t="s">
-        <v>160</v>
+        <v>280</v>
       </c>
       <c r="G6" t="s">
-        <v>167</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1470,16 +2476,16 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>262</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>267</v>
       </c>
       <c r="F7" t="s">
-        <v>161</v>
+        <v>281</v>
       </c>
       <c r="G7" t="s">
-        <v>168</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1487,19 +2493,19 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>263</v>
       </c>
       <c r="D8" t="s">
-        <v>151</v>
+        <v>271</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>276</v>
       </c>
       <c r="F8" t="s">
-        <v>162</v>
+        <v>282</v>
       </c>
       <c r="G8" t="s">
-        <v>169</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -1507,7 +2513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1528,7 +2534,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1543,31 +2549,31 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>174</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>291</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="C8" t="s">
-        <v>177</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1575,7 +2581,7 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>178</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1583,12 +2589,12 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -1596,7 +2602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1633,13 +2639,13 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>298</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>299</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +2653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -1668,7 +2674,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1689,40 +2695,40 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>302</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>307</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>303</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>308</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>245</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>309</v>
       </c>
       <c r="C8" t="s">
-        <v>189</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1743,40 +2749,40 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>186</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>302</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>310</v>
       </c>
       <c r="C12" t="s">
-        <v>200</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>305</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>245</v>
       </c>
       <c r="B14" t="s">
-        <v>193</v>
+        <v>311</v>
       </c>
       <c r="C14" t="s">
-        <v>192</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1797,29 +2803,29 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>188</v>
+        <v>306</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>302</v>
       </c>
       <c r="B18" t="s">
-        <v>194</v>
+        <v>312</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>245</v>
       </c>
       <c r="B19" t="s">
-        <v>194</v>
+        <v>312</v>
       </c>
       <c r="C19" t="s">
-        <v>194</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1840,475 +2846,40 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>302</v>
       </c>
       <c r="B23" t="s">
-        <v>195</v>
+        <v>313</v>
       </c>
       <c r="C23" t="s">
-        <v>201</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>303</v>
       </c>
       <c r="B24" t="s">
-        <v>196</v>
+        <v>314</v>
       </c>
       <c r="C24" t="s">
-        <v>202</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>245</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>315</v>
       </c>
       <c r="C25" t="s">
-        <v>195</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>208</v>
-      </c>
-      <c r="B9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>210</v>
-      </c>
-      <c r="B11" t="s">
-        <v>216</v>
-      </c>
-      <c r="C11" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>211</v>
-      </c>
-      <c r="B12" t="s">
-        <v>217</v>
-      </c>
-      <c r="C12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>208</v>
-      </c>
-      <c r="B13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C13" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>213</v>
-      </c>
-      <c r="B15" t="s">
-        <v>215</v>
-      </c>
-      <c r="C15" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>208</v>
-      </c>
-      <c r="B16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>221</v>
-      </c>
-      <c r="B5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>228</v>
-      </c>
-      <c r="B8" t="s">
-        <v>230</v>
-      </c>
-      <c r="C8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" t="s">
-        <v>231</v>
-      </c>
-      <c r="C9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>237</v>
-      </c>
-      <c r="B4" t="s">
-        <v>239</v>
-      </c>
-      <c r="C4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>242</v>
-      </c>
-      <c r="B6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C7" t="s">
-        <v>247</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -2399,6 +2970,441 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B8" t="s">
+        <v>333</v>
+      </c>
+      <c r="C8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>326</v>
+      </c>
+      <c r="B9" t="s">
+        <v>333</v>
+      </c>
+      <c r="C9" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>328</v>
+      </c>
+      <c r="B11" t="s">
+        <v>334</v>
+      </c>
+      <c r="C11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>329</v>
+      </c>
+      <c r="B12" t="s">
+        <v>335</v>
+      </c>
+      <c r="C12" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>326</v>
+      </c>
+      <c r="B13" t="s">
+        <v>333</v>
+      </c>
+      <c r="C13" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" t="s">
+        <v>333</v>
+      </c>
+      <c r="C15" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>326</v>
+      </c>
+      <c r="B16" t="s">
+        <v>333</v>
+      </c>
+      <c r="C16" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B5" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>344</v>
+      </c>
+      <c r="C6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>345</v>
+      </c>
+      <c r="C7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C9" t="s">
+        <v>354</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>359</v>
+      </c>
+      <c r="B5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>362</v>
+      </c>
+      <c r="C7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
@@ -2563,6 +3569,183 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>2020</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>2020</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2591,16 +3774,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="C2" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2619,16 +3802,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -2639,27 +3822,27 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2667,7 +3850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -2707,46 +3890,46 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2754,7 +3937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2775,7 +3958,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2796,13 +3979,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2810,7 +3993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -2840,24 +4023,24 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2879,277 +4062,224 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="F6" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="F8" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="F13" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="F14" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="F15" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="E16" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="F16" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="F18" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="F19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>